<commit_message>
regionali 2023 nel lazio e in lombardia
aggiunto risultati per liste, preferenze e voti presidente alle elezioni regionali 2023 nel lazio e in lombardia
</commit_message>
<xml_diff>
--- a/dati_disponibili.xlsx
+++ b/dati_disponibili.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="79">
   <si>
     <t>ANNO</t>
   </si>
@@ -106,9 +106,6 @@
     <t>senatori</t>
   </si>
   <si>
-    <t>lista</t>
-  </si>
-  <si>
     <t>[1996 2001 2006 2008 2013 2018 2022]</t>
   </si>
   <si>
@@ -205,7 +202,13 @@
     <t>[2005 2009 2011 2016]</t>
   </si>
   <si>
-    <t>[2005 2010 2013 2018]</t>
+    <t>[2005 2010 2013 2018 2023]</t>
+  </si>
+  <si>
+    <t>[2023]</t>
+  </si>
+  <si>
+    <t>[2018 2023]</t>
   </si>
   <si>
     <t>[2001 2006 2008 2013 2018 2022]</t>
@@ -223,9 +226,6 @@
     <t>[2006]</t>
   </si>
   <si>
-    <t>[2022]</t>
-  </si>
-  <si>
     <t>[2008 2013 2016 2021]</t>
   </si>
   <si>
@@ -235,7 +235,7 @@
     <t>[2021]</t>
   </si>
   <si>
-    <t>[2005 2018]</t>
+    <t>[2005 2018 2023]</t>
   </si>
   <si>
     <t>[2001 2006 2016 2021]</t>
@@ -608,7 +608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -645,7 +645,7 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -660,7 +660,7 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -673,7 +673,7 @@
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -686,7 +686,7 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -697,7 +697,7 @@
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -712,7 +712,7 @@
         <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -723,7 +723,7 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -738,7 +738,7 @@
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -753,7 +753,7 @@
         <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -764,7 +764,7 @@
         <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -775,7 +775,7 @@
         <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -790,7 +790,7 @@
         <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -807,7 +807,7 @@
         <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -822,7 +822,7 @@
         <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -835,7 +835,7 @@
         <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -850,7 +850,7 @@
         <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -865,7 +865,7 @@
         <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -880,7 +880,7 @@
         <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -895,7 +895,7 @@
         <v>24</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -906,7 +906,7 @@
         <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -921,7 +921,7 @@
         <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -938,7 +938,7 @@
         <v>24</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -953,7 +953,7 @@
         <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -964,7 +964,7 @@
         <v>26</v>
       </c>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -975,7 +975,7 @@
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -988,7 +988,7 @@
         <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1003,7 +1003,7 @@
         <v>24</v>
       </c>
       <c r="E28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1014,7 +1014,7 @@
         <v>26</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1029,7 +1029,7 @@
         <v>26</v>
       </c>
       <c r="E30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1040,7 +1040,7 @@
         <v>25</v>
       </c>
       <c r="E31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1053,7 +1053,7 @@
         <v>24</v>
       </c>
       <c r="E32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1064,7 +1064,7 @@
         <v>26</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1079,7 +1079,7 @@
         <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1094,7 +1094,7 @@
         <v>24</v>
       </c>
       <c r="E35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1105,7 +1105,7 @@
         <v>26</v>
       </c>
       <c r="E36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1116,7 +1116,7 @@
         <v>27</v>
       </c>
       <c r="E37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1129,7 +1129,7 @@
         <v>24</v>
       </c>
       <c r="E38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1140,7 +1140,7 @@
         <v>26</v>
       </c>
       <c r="E39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1151,7 +1151,7 @@
         <v>27</v>
       </c>
       <c r="E40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1166,7 +1166,7 @@
         <v>24</v>
       </c>
       <c r="E41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1183,7 +1183,7 @@
         <v>28</v>
       </c>
       <c r="E42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1194,7 +1194,7 @@
         <v>24</v>
       </c>
       <c r="E43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1209,7 +1209,7 @@
         <v>25</v>
       </c>
       <c r="E44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1222,7 +1222,7 @@
         <v>25</v>
       </c>
       <c r="E45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1235,7 +1235,7 @@
         <v>24</v>
       </c>
       <c r="E46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1250,7 +1250,7 @@
         <v>24</v>
       </c>
       <c r="E47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1265,7 +1265,7 @@
         <v>24</v>
       </c>
       <c r="E48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1276,7 +1276,7 @@
         <v>27</v>
       </c>
       <c r="E49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1291,7 +1291,7 @@
         <v>24</v>
       </c>
       <c r="E50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1304,7 +1304,7 @@
         <v>24</v>
       </c>
       <c r="E51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1319,7 +1319,7 @@
         <v>19</v>
       </c>
       <c r="E52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1334,22 +1334,18 @@
         <v>24</v>
       </c>
       <c r="E53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1"/>
-      <c r="B54" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E54" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1357,18 +1353,16 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E55" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A56" s="1"/>
       <c r="B56" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>21</v>
@@ -1377,28 +1371,26 @@
         <v>24</v>
       </c>
       <c r="E56" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1"/>
-      <c r="B57" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E57" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B58" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>21</v>
@@ -1413,7 +1405,7 @@
     <row r="59" spans="1:5">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>22</v>
@@ -1422,45 +1414,45 @@
         <v>24</v>
       </c>
       <c r="E59" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E60" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E61" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="1"/>
+      <c r="A62" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B62" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>21</v>
@@ -1473,53 +1465,59 @@
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E63" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
+      <c r="B64" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D64" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E64" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="1"/>
+      <c r="A65" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B65" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E65" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
+      <c r="B66" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C66" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>25</v>
@@ -1532,204 +1530,202 @@
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
+      <c r="C68" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D68" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E68" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="1"/>
-      <c r="B69" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E69" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="1"/>
       <c r="B70" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E70" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
+      <c r="B71" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C71" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E71" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E72" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
+      <c r="C73" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D73" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E73" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="1"/>
-      <c r="B74" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E74" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
+      <c r="B75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D75" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E75" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E76" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1"/>
-      <c r="B77" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E77" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
+      <c r="A78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D78" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E78" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
+      <c r="B79" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="C79" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E79" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
-      <c r="C80" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E80" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
+      <c r="C81" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D81" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E81" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="1"/>
-      <c r="B82" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
         <v>21</v>
       </c>
@@ -1737,89 +1733,115 @@
         <v>24</v>
       </c>
       <c r="E82" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="1"/>
-      <c r="B83" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E83" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
+      <c r="B84" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D84" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E84" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="1"/>
       <c r="B85" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E85" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="1"/>
-      <c r="B86" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E86" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
+      <c r="B87" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D87" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E87" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="1"/>
       <c r="B88" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E88" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E89" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E88" t="s">
-        <v>54</v>
+      <c r="C90" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E90" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1827,11 +1849,11 @@
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="A14:A22"/>
     <mergeCell ref="A23:A41"/>
-    <mergeCell ref="A42:A55"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A63:A75"/>
-    <mergeCell ref="A76:A88"/>
+    <mergeCell ref="A42:A57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="A65:A77"/>
+    <mergeCell ref="A78:A90"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B10:B12"/>
@@ -1845,14 +1867,14 @@
     <mergeCell ref="B44:B46"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="B88:B89"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C10:C12"/>
@@ -1865,15 +1887,15 @@
     <mergeCell ref="C38:C40"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="C75:C77"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C88:C89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Napoli ed Europee 2024
aggiunto shapefile di napoli ed elezioni europee 2024
</commit_message>
<xml_diff>
--- a/dati_disponibili.xlsx
+++ b/dati_disponibili.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="86">
   <si>
     <t>ANNO</t>
   </si>
@@ -31,6 +31,9 @@
     <t>liste_sindaco_preferenze_referendum_presidente</t>
   </si>
   <si>
+    <t>BARI</t>
+  </si>
+  <si>
     <t>BOLOGNA</t>
   </si>
   <si>
@@ -52,18 +55,21 @@
     <t>ROMA</t>
   </si>
   <si>
+    <t>TARANTO</t>
+  </si>
+  <si>
     <t>TORINO</t>
   </si>
   <si>
     <t>camera</t>
   </si>
   <si>
+    <t>europee</t>
+  </si>
+  <si>
     <t>comunali</t>
   </si>
   <si>
-    <t>europee</t>
-  </si>
-  <si>
     <t>municipali</t>
   </si>
   <si>
@@ -79,6 +85,9 @@
     <t>provinciali</t>
   </si>
   <si>
+    <t>comune</t>
+  </si>
+  <si>
     <t>single-round</t>
   </si>
   <si>
@@ -106,6 +115,12 @@
     <t>senatori</t>
   </si>
   <si>
+    <t>[2022]</t>
+  </si>
+  <si>
+    <t>[2019 2024]</t>
+  </si>
+  <si>
     <t>[1996 2001 2006 2008 2013 2018 2022]</t>
   </si>
   <si>
@@ -118,7 +133,7 @@
     <t>[1999 2004 2009 2011 2014 2016 2021]</t>
   </si>
   <si>
-    <t>[1994 1999 2009 2014 2019]</t>
+    <t>[1994 1999 2009 2014 2019 2024]</t>
   </si>
   <si>
     <t>[1999 2009 2014 2019]</t>
@@ -142,6 +157,9 @@
     <t>[2009 2014 2019]</t>
   </si>
   <si>
+    <t>[2014 2019 2024]</t>
+  </si>
+  <si>
     <t>[2019]</t>
   </si>
   <si>
@@ -163,6 +181,9 @@
     <t>[2017]</t>
   </si>
   <si>
+    <t>[2009 2014 2019 2024]</t>
+  </si>
+  <si>
     <t>[2012]</t>
   </si>
   <si>
@@ -190,7 +211,7 @@
     <t>[2011 2016 2021]</t>
   </si>
   <si>
-    <t>[2004 2009 2014 2019]</t>
+    <t>[2004 2009 2014 2019 2024]</t>
   </si>
   <si>
     <t>[2009]</t>
@@ -214,7 +235,7 @@
     <t>[2001 2006 2008 2013 2018 2022]</t>
   </si>
   <si>
-    <t>[2004 2009 2019]</t>
+    <t>[2004 2009 2019 2024]</t>
   </si>
   <si>
     <t>[2005 2010 2015 2020]</t>
@@ -608,7 +629,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -636,83 +657,89 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -720,10 +747,10 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -732,289 +759,289 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D25" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D26" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1"/>
-      <c r="B28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D29" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1023,13 +1050,13 @@
         <v>16</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E30" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1037,23 +1064,25 @@
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C32" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E32" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1061,75 +1090,75 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E33" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1"/>
-      <c r="B34" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E34" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1"/>
-      <c r="B35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E35" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D36" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E36" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D37" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E37" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E38" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1137,241 +1166,239 @@
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E39" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D40" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E40" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1"/>
-      <c r="B41" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E41" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E42" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D43" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E43" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B44" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E44" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E45" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C46" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E46" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1"/>
-      <c r="B47" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E47" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1"/>
-      <c r="B48" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E48" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D49" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E49" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E50" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E51" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E52" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1"/>
-      <c r="B53" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E53" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D54" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E54" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
+      <c r="B55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D55" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E55" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1"/>
-      <c r="B56" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E56" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1379,57 +1406,53 @@
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E57" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E58" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1"/>
-      <c r="B59" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E59" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="1"/>
+      <c r="A60" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B60" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E60" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1438,60 +1461,56 @@
         <v>17</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E61" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E62" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1"/>
-      <c r="B63" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E63" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E64" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1499,204 +1518,212 @@
         <v>11</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E65" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1"/>
       <c r="B66" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E66" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
+      <c r="B67" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C67" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E67" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
+      <c r="B68" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C68" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E68" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
+      <c r="A69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D69" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E69" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="1"/>
       <c r="B70" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E70" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="1"/>
-      <c r="B71" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E71" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E72" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
-      <c r="C73" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E73" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
+      <c r="B74" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D74" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E74" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="1"/>
       <c r="B75" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E75" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
+      <c r="C76" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D76" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E76" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
+      <c r="C77" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D77" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E77" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E78" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="1"/>
       <c r="B79" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E79" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -1704,62 +1731,68 @@
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E80" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
-      <c r="C81" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E81" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E82" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E82" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
+      <c r="B83" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D83" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E83" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="1"/>
       <c r="B84" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E84" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1768,39 +1801,45 @@
         <v>16</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E85" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
+      <c r="B86" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D86" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E86" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="1"/>
+      <c r="A87" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B87" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E87" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -1809,13 +1848,13 @@
         <v>17</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E88" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -1823,79 +1862,201 @@
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E89" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="1"/>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="1"/>
+      <c r="C90" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E90" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E91" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E92" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E93" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E90" t="s">
-        <v>53</v>
+      <c r="C94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E94" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E95" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E96" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E97" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E98" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E99" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="50">
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A22"/>
-    <mergeCell ref="A23:A41"/>
-    <mergeCell ref="A42:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="A65:A77"/>
-    <mergeCell ref="A78:A90"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B48:B49"/>
+  <mergeCells count="53">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A15"/>
+    <mergeCell ref="A16:A24"/>
+    <mergeCell ref="A25:A43"/>
+    <mergeCell ref="A44:A59"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A69:A81"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A99"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B46:B48"/>
     <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="B88:B92"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="B97:B98"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C26:C28"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="C75:C77"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C81"/>
     <mergeCell ref="C88:C89"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C97:C98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>